<commit_message>
added test method for class EquilateralTriangle with wrong triangle type values
</commit_message>
<xml_diff>
--- a/DEV-12/DataSources/DataForEquilateralTriangle.xlsx
+++ b/DEV-12/DataSources/DataForEquilateralTriangle.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Valid" sheetId="1" r:id="rId1"/>
     <sheet name="Invalid" sheetId="2" r:id="rId2"/>
     <sheet name="WrongFormat" sheetId="3" r:id="rId3"/>
+    <sheet name="WrongType" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="24">
   <si>
     <t>SideA</t>
   </si>
@@ -79,6 +80,15 @@
   </si>
   <si>
     <t>0.1</t>
+  </si>
+  <si>
+    <t>0,000011</t>
+  </si>
+  <si>
+    <t>0,000012</t>
+  </si>
+  <si>
+    <t>0,000013</t>
   </si>
 </sst>
 </file>
@@ -129,7 +139,19 @@
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="16">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
@@ -177,8 +199,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Таблица1" displayName="Таблица1" ref="A1:C10" totalsRowShown="0" dataDxfId="11">
-  <autoFilter ref="A1:C10"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Таблица1" displayName="Таблица1" ref="A1:C11" totalsRowShown="0" dataDxfId="15">
+  <autoFilter ref="A1:C11"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="SideA" dataDxfId="14"/>
+    <tableColumn id="2" name="SideB" dataDxfId="13"/>
+    <tableColumn id="3" name="SideC" dataDxfId="12"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Таблица2" displayName="Таблица2" ref="A1:C8" totalsRowShown="0" dataDxfId="11">
+  <autoFilter ref="A1:C8"/>
   <tableColumns count="3">
     <tableColumn id="1" name="SideA" dataDxfId="10"/>
     <tableColumn id="2" name="SideB" dataDxfId="9"/>
@@ -188,9 +222,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Таблица2" displayName="Таблица2" ref="A1:C8" totalsRowShown="0" dataDxfId="7">
-  <autoFilter ref="A1:C8"/>
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Таблица3" displayName="Таблица3" ref="A1:C4" totalsRowShown="0" dataDxfId="7">
+  <autoFilter ref="A1:C4"/>
   <tableColumns count="3">
     <tableColumn id="1" name="SideA" dataDxfId="6"/>
     <tableColumn id="2" name="SideB" dataDxfId="5"/>
@@ -200,9 +234,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Таблица3" displayName="Таблица3" ref="A1:C4" totalsRowShown="0" dataDxfId="0">
-  <autoFilter ref="A1:C4"/>
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Таблица4" displayName="Таблица4" ref="A1:C10" totalsRowShown="0" dataDxfId="0">
+  <autoFilter ref="A1:C10"/>
   <tableColumns count="3">
     <tableColumn id="1" name="SideA" dataDxfId="3"/>
     <tableColumn id="2" name="SideB" dataDxfId="2"/>
@@ -499,10 +533,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,44 +578,44 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+      <c r="A4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
         <v>0.1</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B5" s="1">
         <v>0.1</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C5" s="1">
         <v>0.1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>4</v>
@@ -592,18 +626,18 @@
         <v>3</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>3</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>3</v>
@@ -611,12 +645,23 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -757,7 +802,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
@@ -816,4 +861,135 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="11.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1">
+        <v>3</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>3</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>3</v>
+      </c>
+      <c r="B10" s="1">
+        <v>2</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added test classes for triangle builders
</commit_message>
<xml_diff>
--- a/DEV-12/DataSources/DataForEquilateralTriangle.xlsx
+++ b/DEV-12/DataSources/DataForEquilateralTriangle.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Valid" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="28">
   <si>
     <t>SideA</t>
   </si>
@@ -89,13 +89,25 @@
   </si>
   <si>
     <t>0,000013</t>
+  </si>
+  <si>
+    <t>double_Max_value</t>
+  </si>
+  <si>
+    <t>double_Min_value</t>
+  </si>
+  <si>
+    <t>1,7976931348623157E+308</t>
+  </si>
+  <si>
+    <t>-1,7976931348623157E+308</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -109,6 +121,14 @@
       <name val="Segoe UI"/>
       <family val="2"/>
       <charset val="204"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF2A2A2A"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -131,10 +151,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -211,8 +232,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Таблица2" displayName="Таблица2" ref="A1:C8" totalsRowShown="0" dataDxfId="11">
-  <autoFilter ref="A1:C8"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Таблица2" displayName="Таблица2" ref="A1:C10" totalsRowShown="0" dataDxfId="11">
+  <autoFilter ref="A1:C10"/>
   <tableColumns count="3">
     <tableColumn id="1" name="SideA" dataDxfId="10"/>
     <tableColumn id="2" name="SideB" dataDxfId="9"/>
@@ -235,12 +256,12 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Таблица4" displayName="Таблица4" ref="A1:C10" totalsRowShown="0" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Таблица4" displayName="Таблица4" ref="A1:C10" totalsRowShown="0" dataDxfId="3">
   <autoFilter ref="A1:C10"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="SideA" dataDxfId="3"/>
-    <tableColumn id="2" name="SideB" dataDxfId="2"/>
-    <tableColumn id="3" name="SideC" dataDxfId="1"/>
+    <tableColumn id="1" name="SideA" dataDxfId="2"/>
+    <tableColumn id="2" name="SideB" dataDxfId="1"/>
+    <tableColumn id="3" name="SideC" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -535,7 +556,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -675,10 +696,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -787,6 +808,34 @@
       </c>
       <c r="D8" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>